<commit_message>
Renamed server.js to appease the google cloud deities
</commit_message>
<xml_diff>
--- a/updated.xlsx
+++ b/updated.xlsx
@@ -398,6 +398,65 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Street</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Town</v>
+      </c>
+      <c r="C1" t="str">
+        <v>State</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>408 Salerno Way</v>
+      </c>
+      <c r="B2" t="str">
+        <v>Howell</v>
+      </c>
+      <c r="C2" t="str">
+        <v>NJ</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>1967 Pennington Rd</v>
+      </c>
+      <c r="B3" t="str">
+        <v>Ewing</v>
+      </c>
+      <c r="C3" t="str">
+        <v>NJ</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>408 Salerno Way</v>
+      </c>
+      <c r="B4" t="str">
+        <v>Howell</v>
+      </c>
+      <c r="C4" t="str">
+        <v>NJ</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:C4"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
@@ -476,63 +535,4 @@
     <ignoredError numberStoredAsText="1" sqref="A1:E4"/>
   </ignoredErrors>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0" rightToLeft="0"/>
-  </sheetViews>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>Street</v>
-      </c>
-      <c r="B1" t="str">
-        <v>Town</v>
-      </c>
-      <c r="C1" t="str">
-        <v>State</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>408 Salerno Way</v>
-      </c>
-      <c r="B2" t="str">
-        <v>Howell</v>
-      </c>
-      <c r="C2" t="str">
-        <v>NJ</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>1967 Pennington Rd</v>
-      </c>
-      <c r="B3" t="str">
-        <v>Ewing</v>
-      </c>
-      <c r="C3" t="str">
-        <v>NJ</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>408 Salerno Way</v>
-      </c>
-      <c r="B4" t="str">
-        <v>Howell</v>
-      </c>
-      <c r="C4" t="str">
-        <v>NJ</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C4"/>
-  </ignoredErrors>
-</worksheet>
 </file>
</xml_diff>